<commit_message>
update results hierarchical full sample
</commit_message>
<xml_diff>
--- a/output/results/results hierarchichal vs bisg full_sample.xlsx
+++ b/output/results/results hierarchichal vs bisg full_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamariapatron/Desktop/GRI/cascade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECC9B13-8AB6-944A-B839-254F11DCB003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47789F7-570D-FD4C-91C2-CE793DA10FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="0" windowWidth="22720" windowHeight="18000" activeTab="1" xr2:uid="{11842B35-267D-CF4B-A691-2EFF1C0A1132}"/>
+    <workbookView xWindow="6080" yWindow="0" windowWidth="22720" windowHeight="18000" xr2:uid="{11842B35-267D-CF4B-A691-2EFF1C0A1132}"/>
   </bookViews>
   <sheets>
     <sheet name="confusion matrix" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6381FF8D-2B62-A64E-9916-093C2BDB691A}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -805,19 +805,10 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>2829</v>
-      </c>
-      <c r="D15">
-        <v>902</v>
-      </c>
-      <c r="E15">
-        <v>269</v>
+        <v>3853</v>
       </c>
       <c r="F15">
-        <v>604</v>
-      </c>
-      <c r="G15">
-        <v>1250</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -826,19 +817,10 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>31</v>
-      </c>
-      <c r="D16">
-        <v>16084</v>
-      </c>
-      <c r="E16">
-        <v>272</v>
+        <v>3131</v>
       </c>
       <c r="F16">
-        <v>1122</v>
-      </c>
-      <c r="G16">
-        <v>1153</v>
+        <v>15531</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -849,19 +831,10 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>349</v>
-      </c>
-      <c r="E17">
-        <v>7712</v>
+        <v>78</v>
       </c>
       <c r="F17">
-        <v>1429</v>
-      </c>
-      <c r="G17">
-        <v>2266</v>
+        <v>11688</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -870,19 +843,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>195</v>
-      </c>
-      <c r="D18">
-        <v>4752</v>
-      </c>
-      <c r="E18">
-        <v>10743</v>
+        <v>571</v>
       </c>
       <c r="F18">
-        <v>29894</v>
-      </c>
-      <c r="G18">
-        <v>11732</v>
+        <v>56745</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -891,19 +855,10 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>173</v>
-      </c>
-      <c r="D19">
-        <v>1227</v>
-      </c>
-      <c r="E19">
-        <v>556</v>
+        <v>595</v>
       </c>
       <c r="F19">
-        <v>2121</v>
-      </c>
-      <c r="G19">
-        <v>1353</v>
+        <v>4835</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -952,7 +907,7 @@
         <v>2829</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>902</v>
       </c>
       <c r="E25">
         <v>269</v>
@@ -961,7 +916,7 @@
         <v>604</v>
       </c>
       <c r="G25">
-        <v>2152</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -973,7 +928,7 @@
         <v>31</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>16084</v>
       </c>
       <c r="E26">
         <v>272</v>
@@ -982,7 +937,7 @@
         <v>1122</v>
       </c>
       <c r="G26">
-        <v>17237</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -996,7 +951,7 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>349</v>
       </c>
       <c r="E27">
         <v>7712</v>
@@ -1005,7 +960,7 @@
         <v>1429</v>
       </c>
       <c r="G27">
-        <v>2615</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1017,7 +972,7 @@
         <v>195</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>4752</v>
       </c>
       <c r="E28">
         <v>10743</v>
@@ -1026,7 +981,7 @@
         <v>29894</v>
       </c>
       <c r="G28">
-        <v>16484</v>
+        <v>11732</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1038,7 +993,7 @@
         <v>173</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1227</v>
       </c>
       <c r="E29">
         <v>556</v>
@@ -1047,7 +1002,7 @@
         <v>2121</v>
       </c>
       <c r="G29">
-        <v>2580</v>
+        <v>1353</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9625C5-279F-2E41-A596-3DCFD1F5B6BF}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hierarchical, tract level, for full dataset
</commit_message>
<xml_diff>
--- a/output/results/results hierarchichal vs bisg full_sample.xlsx
+++ b/output/results/results hierarchichal vs bisg full_sample.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamariapatron/Desktop/GRI/cascade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47789F7-570D-FD4C-91C2-CE793DA10FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8B03EF-5563-CF49-9D57-5FA084403E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="0" windowWidth="22720" windowHeight="18000" xr2:uid="{11842B35-267D-CF4B-A691-2EFF1C0A1132}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{11842B35-267D-CF4B-A691-2EFF1C0A1132}"/>
   </bookViews>
   <sheets>
-    <sheet name="confusion matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="metrics" sheetId="2" r:id="rId2"/>
+    <sheet name="CMcounty" sheetId="1" r:id="rId1"/>
+    <sheet name="metrics_county" sheetId="2" r:id="rId2"/>
+    <sheet name="CMtract" sheetId="3" r:id="rId3"/>
+    <sheet name="metrics_tract" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="24">
   <si>
     <t>PREDICTED</t>
   </si>
@@ -99,10 +101,16 @@
     <t>hierarchical: multypling leafs</t>
   </si>
   <si>
-    <t>metrics for subsampe of 99 observations. County level, only surname</t>
-  </si>
-  <si>
     <t>confusion matrix for full sample. County level, only surname</t>
+  </si>
+  <si>
+    <t>metrics for fullsample. County level, only surname</t>
+  </si>
+  <si>
+    <t>confusion matrix for full sample. Tract_level, only surname</t>
+  </si>
+  <si>
+    <t>metrics for full_sample. Tract level, only surname</t>
   </si>
 </sst>
 </file>
@@ -280,6 +288,84 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD5C0EDB-409D-1B48-923F-D20B3B633BA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6718300" y="596900"/>
+          <a:ext cx="7086600" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>there</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -607,15 +693,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6381FF8D-2B62-A64E-9916-093C2BDB691A}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1021,7 +1107,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1119,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1277,6 +1363,687 @@
       </c>
       <c r="D27">
         <v>7.6208178438661706E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D2E7C1-6835-D54E-88BD-C2C2FC696365}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3378</v>
+      </c>
+      <c r="D5">
+        <v>659</v>
+      </c>
+      <c r="E5">
+        <v>111</v>
+      </c>
+      <c r="F5">
+        <v>1643</v>
+      </c>
+      <c r="G5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>15700</v>
+      </c>
+      <c r="E6">
+        <v>177</v>
+      </c>
+      <c r="F6">
+        <v>2589</v>
+      </c>
+      <c r="G6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>78</v>
+      </c>
+      <c r="E7">
+        <v>5608</v>
+      </c>
+      <c r="F7">
+        <v>5988</v>
+      </c>
+      <c r="G7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>283</v>
+      </c>
+      <c r="D8">
+        <v>915</v>
+      </c>
+      <c r="E8">
+        <v>2229</v>
+      </c>
+      <c r="F8">
+        <v>53623</v>
+      </c>
+      <c r="G8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>321</v>
+      </c>
+      <c r="D9">
+        <v>486</v>
+      </c>
+      <c r="E9">
+        <v>297</v>
+      </c>
+      <c r="F9">
+        <v>4137</v>
+      </c>
+      <c r="G9">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>4039</v>
+      </c>
+      <c r="F15">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>3048</v>
+      </c>
+      <c r="F16">
+        <v>15614</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+      <c r="F17">
+        <v>11616</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>752</v>
+      </c>
+      <c r="F18">
+        <v>56564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>617</v>
+      </c>
+      <c r="F19">
+        <v>4813</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>2850</v>
+      </c>
+      <c r="D25">
+        <v>984</v>
+      </c>
+      <c r="E25">
+        <v>210</v>
+      </c>
+      <c r="F25">
+        <v>572</v>
+      </c>
+      <c r="G25">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>32</v>
+      </c>
+      <c r="D26">
+        <v>16406</v>
+      </c>
+      <c r="E26">
+        <v>153</v>
+      </c>
+      <c r="F26">
+        <v>793</v>
+      </c>
+      <c r="G26">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>261</v>
+      </c>
+      <c r="E27">
+        <v>7272</v>
+      </c>
+      <c r="F27">
+        <v>1479</v>
+      </c>
+      <c r="G27">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>234</v>
+      </c>
+      <c r="D28">
+        <v>2547</v>
+      </c>
+      <c r="E28">
+        <v>6788</v>
+      </c>
+      <c r="F28">
+        <v>35744</v>
+      </c>
+      <c r="G28">
+        <v>11862</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>178</v>
+      </c>
+      <c r="D29">
+        <v>801</v>
+      </c>
+      <c r="E29">
+        <v>436</v>
+      </c>
+      <c r="F29">
+        <v>2350</v>
+      </c>
+      <c r="G29">
+        <v>1647</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C22:E22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8106DC6E-F050-2742-AC72-2E61A435E5FB}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.87980000000000003</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.87380000000000002</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.89359999999999995</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.64039999999999997</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.91069999999999995</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.96479999999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.58989999999999998</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.60270000000000001</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>0.937874945343244</v>
+      </c>
+      <c r="C15">
+        <v>0.98688237866200301</v>
+      </c>
+      <c r="D15">
+        <v>0.62516834280717104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>0.47691130198146098</v>
+      </c>
+      <c r="D16">
+        <v>0.61841993366782899</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0.57822663471413904</v>
+      </c>
+      <c r="C17">
+        <v>0.69085929476206798</v>
+      </c>
+      <c r="D17">
+        <v>0.48784662786716898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>0.841732790049324</v>
+      </c>
+      <c r="D18">
+        <v>0.87958395882479101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>3.1596452328159601E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.30432372505543198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>0.78880553103854101</v>
+      </c>
+      <c r="C23">
+        <v>0.62528396812907905</v>
+      </c>
+      <c r="D23">
+        <v>0.87312521373784702</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>0.66587508905248205</v>
+      </c>
+      <c r="D24">
+        <v>0.48940036341611098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>0.81771968046477805</v>
+      </c>
+      <c r="C25">
+        <v>0.46924776188815298</v>
+      </c>
+      <c r="D25">
+        <v>0.86259079903147695</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>0.88014351384684397</v>
+      </c>
+      <c r="D26">
+        <v>0.78127529882375302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>0.36460554371002102</v>
+      </c>
+      <c r="D27">
+        <v>8.7886872998932802E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>